<commit_message>
Added function to join calib. & valid. data sheets
Signed-off-by: Dimitri Lezcano <dlezcan1@jhu.edu>
</commit_message>
<xml_diff>
--- a/FBG_Needle_Calibration_Data/needle_3CH_4AA/Validation_Jig_Calibration_08-19-20/Validation_Error.xlsx
+++ b/FBG_Needle_Calibration_Data/needle_3CH_4AA/Validation_Jig_Calibration_08-19-20/Validation_Error.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\AMIRo\FBG_Needle_Calibration_Data\needle_3CH_4AA\Validation_Jig_Calibration_08-19-20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2813CA5D-BEF1-4411-BE59-84EC07839720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE989900-C8DF-4CB4-8D63-83AFD79035AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="23610" windowHeight="12930" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="2715" windowWidth="23610" windowHeight="12930" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AA1" sheetId="1" r:id="rId1"/>
-    <sheet name="AA2" sheetId="8" r:id="rId2"/>
-    <sheet name="AA3" sheetId="9" r:id="rId3"/>
-    <sheet name="AA4" sheetId="10" r:id="rId4"/>
+    <sheet name="AA2" sheetId="11" r:id="rId2"/>
+    <sheet name="AA3" sheetId="12" r:id="rId3"/>
+    <sheet name="AA4" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -2122,7 +2122,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Curv. Y (0 deg)</c:v>
+            <c:v>Curv. Y (In-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2211,7 +2211,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Curv. X (0 deg)</c:v>
+            <c:v>Curv. X (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -2297,10 +2297,99 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="3"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Curv. Y (90 deg)</c:v>
+            <c:v>Curv. X (In-Plane)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'AA1'!$B$10:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'AA1'!$J$10:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5463245102900598E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1592517266939146</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7462179741477799E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16871512517046081</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3272610616421389E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-75D5-4990-B678-121231878A1B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Curv. Y (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -2379,95 +2468,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-75D5-4990-B678-121231878A1B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Curv. X (90 deg)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'AA1'!$B$10:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'AA1'!$J$10:$J$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.5463245102900598E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1592517266939146</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.7462179741477799E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.16871512517046081</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3272610616421389E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-75D5-4990-B678-121231878A1B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2820,7 +2820,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Angular</a:t>
+              <a:t>Curvature</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -2828,8 +2828,15 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>: Predicted vs. Actual</a:t>
+              <a:t>: </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Out-of-Plane</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2869,13 +2876,13 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>0 deg</c:v>
+            <c:v>Curv. X (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2886,11 +2893,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2898,7 +2905,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'AA1'!$D$4:$D$9</c:f>
+              <c:f>'AA1'!$C$4:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2906,26 +2913,26 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>-0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>-0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25</c:v>
+                  <c:v>-1.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.125</c:v>
+                  <c:v>-3.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'AA1'!$O$4:$O$9</c:f>
+              <c:f>'AA1'!$J$4:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2933,19 +2940,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.5822145449822713</c:v>
+                  <c:v>-2.6515408016102051E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.4200102257793499</c:v>
+                  <c:v>3.6451250803679711E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.209380916785491</c:v>
+                  <c:v>-3.4955612165494879E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.7255815222641724</c:v>
+                  <c:v>-0.1076257727980859</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.8243495732552741</c:v>
+                  <c:v>-0.14832148453655011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2953,7 +2960,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2573-4C6D-9EEF-9B9E5A2B6C15}"/>
+              <c16:uniqueId val="{00000001-3A14-412A-8ACB-54897D9A86C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2961,7 +2968,7 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>90 deg</c:v>
+            <c:v>Curv. Y (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -2987,7 +2994,31 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'AA1'!$D$10:$D$15</c:f>
+              <c:f>'AA1'!$B$11:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'AA1'!$K$10:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2995,46 +3026,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>-1.170563399185243E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>5.7767248365948078E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>2.93498664108722E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25</c:v>
+                  <c:v>-3.152053401808827E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'AA1'!$O$10:$O$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0693359572203169</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-5.151626061003423</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-1.728583922838471</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.669756327644188</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.6331868910128671</c:v>
+                  <c:v>-8.8437106038202748E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3042,7 +3046,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-2573-4C6D-9EEF-9B9E5A2B6C15}"/>
+              <c16:uniqueId val="{00000003-3A14-412A-8ACB-54897D9A86C9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3202,19 +3206,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Arg Error (degs)</a:t>
+                  <a:t>Predicted Curvature Error (1/m)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="2.5000000000000001E-2"/>
-              <c:y val="0.38930555555555557"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3518,7 +3514,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D621-43DC-B1DA-A53CE7BBFFB8}"/>
+              <c16:uniqueId val="{00000000-A80C-4A8A-B78D-75F9C9B1CA08}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3643,7 +3639,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D621-43DC-B1DA-A53CE7BBFFB8}"/>
+              <c16:uniqueId val="{00000001-A80C-4A8A-B78D-75F9C9B1CA08}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4111,7 +4107,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-601D-45F0-8D81-0F204E405551}"/>
+              <c16:uniqueId val="{00000000-8271-46C6-AAAD-CFEF7F300E0E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4236,7 +4232,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-601D-45F0-8D81-0F204E405551}"/>
+              <c16:uniqueId val="{00000001-8271-46C6-AAAD-CFEF7F300E0E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4704,7 +4700,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7734-4C5E-B138-30DF031CE9B3}"/>
+              <c16:uniqueId val="{00000000-B838-4A08-83EC-072E35D01D92}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4829,7 +4825,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7734-4C5E-B138-30DF031CE9B3}"/>
+              <c16:uniqueId val="{00000001-B838-4A08-83EC-072E35D01D92}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5315,7 +5311,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-60B3-460A-986D-7E4C85C4918A}"/>
+              <c16:uniqueId val="{00000000-CF14-4108-BFA3-131FF2226271}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5404,7 +5400,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-60B3-460A-986D-7E4C85C4918A}"/>
+              <c16:uniqueId val="{00000001-CF14-4108-BFA3-131FF2226271}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5493,7 +5489,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-60B3-460A-986D-7E4C85C4918A}"/>
+              <c16:uniqueId val="{00000002-CF14-4108-BFA3-131FF2226271}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5582,7 +5578,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-60B3-460A-986D-7E4C85C4918A}"/>
+              <c16:uniqueId val="{00000003-CF14-4108-BFA3-131FF2226271}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6068,7 +6064,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3AE4-44B7-B4FB-A6D5F62DAFCA}"/>
+              <c16:uniqueId val="{00000000-435D-481B-A912-487CADEA576B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6157,7 +6153,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3AE4-44B7-B4FB-A6D5F62DAFCA}"/>
+              <c16:uniqueId val="{00000001-435D-481B-A912-487CADEA576B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6243,7 +6239,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3AE4-44B7-B4FB-A6D5F62DAFCA}"/>
+              <c16:uniqueId val="{00000002-435D-481B-A912-487CADEA576B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6332,7 +6328,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-3AE4-44B7-B4FB-A6D5F62DAFCA}"/>
+              <c16:uniqueId val="{00000003-435D-481B-A912-487CADEA576B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6823,7 +6819,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-78AF-48DC-9F50-3D5BB7ABD709}"/>
+              <c16:uniqueId val="{00000000-C13C-4AC4-AEA4-C6BD664554E4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6912,7 +6908,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-78AF-48DC-9F50-3D5BB7ABD709}"/>
+              <c16:uniqueId val="{00000001-C13C-4AC4-AEA4-C6BD664554E4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7001,7 +6997,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-78AF-48DC-9F50-3D5BB7ABD709}"/>
+              <c16:uniqueId val="{00000002-C13C-4AC4-AEA4-C6BD664554E4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7090,7 +7086,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-78AF-48DC-9F50-3D5BB7ABD709}"/>
+              <c16:uniqueId val="{00000003-C13C-4AC4-AEA4-C6BD664554E4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8169,7 +8165,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5489-4F6A-BDBA-74F93AD168FE}"/>
+              <c16:uniqueId val="{00000000-3D4E-45E6-8206-601654F568CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8258,7 +8254,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5489-4F6A-BDBA-74F93AD168FE}"/>
+              <c16:uniqueId val="{00000001-3D4E-45E6-8206-601654F568CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8734,7 +8730,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EAA6-46B5-9210-D88D275BBEE3}"/>
+              <c16:uniqueId val="{00000000-5ED6-4E34-9351-5A826A64D189}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8859,7 +8855,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EAA6-46B5-9210-D88D275BBEE3}"/>
+              <c16:uniqueId val="{00000001-5ED6-4E34-9351-5A826A64D189}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9327,7 +9323,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-678C-4C56-8BB8-F736B88B60D8}"/>
+              <c16:uniqueId val="{00000000-C545-4384-8435-E5414CC9713A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9452,7 +9448,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-678C-4C56-8BB8-F736B88B60D8}"/>
+              <c16:uniqueId val="{00000001-C545-4384-8435-E5414CC9713A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9900,7 +9896,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-489E-4E81-89F9-C840FBD29576}"/>
+              <c16:uniqueId val="{00000000-43D8-4E04-9A33-B3A32AE28469}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -9989,7 +9985,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-489E-4E81-89F9-C840FBD29576}"/>
+              <c16:uniqueId val="{00000001-43D8-4E04-9A33-B3A32AE28469}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10065,7 +10061,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-489E-4E81-89F9-C840FBD29576}"/>
+              <c16:uniqueId val="{00000002-43D8-4E04-9A33-B3A32AE28469}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10475,7 +10471,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-929C-4F45-9DC9-8A0E8D7E71FB}"/>
+              <c16:uniqueId val="{00000000-26CD-4CE8-8620-784921924358}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10564,7 +10560,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-929C-4F45-9DC9-8A0E8D7E71FB}"/>
+              <c16:uniqueId val="{00000001-26CD-4CE8-8620-784921924358}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10653,7 +10649,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-929C-4F45-9DC9-8A0E8D7E71FB}"/>
+              <c16:uniqueId val="{00000002-26CD-4CE8-8620-784921924358}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10742,7 +10738,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-929C-4F45-9DC9-8A0E8D7E71FB}"/>
+              <c16:uniqueId val="{00000003-26CD-4CE8-8620-784921924358}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11154,7 +11150,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Curv. Y (0 deg)</c:v>
+            <c:v>Curv. Y (In-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -11235,7 +11231,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0444-41E3-9453-264511DD6638}"/>
+              <c16:uniqueId val="{00000000-4645-494C-9E97-96BB025BD3AE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11243,7 +11239,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Curv. X (0 deg)</c:v>
+            <c:v>Curv. X (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -11324,15 +11320,104 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0444-41E3-9453-264511DD6638}"/>
+              <c16:uniqueId val="{00000001-4645-494C-9E97-96BB025BD3AE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Curv. X (In-Plane)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'AA2'!$B$10:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'AA2'!$J$10:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.8688453014125968E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.7800227472624133E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-4.0585528002521583E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-9.1227458650831927E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.7281119532911262E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4645-494C-9E97-96BB025BD3AE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
-            <c:v>Curv. Y (90 deg)</c:v>
+            <c:v>Curv. Y (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -11410,96 +11495,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0444-41E3-9453-264511DD6638}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Curv. X (90 deg)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'AA2'!$B$10:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'AA2'!$J$10:$J$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-1.8688453014125968E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-3.7800227472624133E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-4.0585528002521583E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-9.1227458650831927E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-5.7281119532911262E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-0444-41E3-9453-264511DD6638}"/>
+              <c16:uniqueId val="{00000003-4645-494C-9E97-96BB025BD3AE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11852,7 +11848,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Angular</a:t>
+              <a:t>Curvature</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -11860,8 +11856,15 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>: Predicted vs. Actual</a:t>
+              <a:t>: </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Out-of-Plane</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -11901,13 +11904,13 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>0 deg</c:v>
+            <c:v>Curv. X (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -11918,11 +11921,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -11930,7 +11933,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'AA2'!$D$4:$D$9</c:f>
+              <c:f>'AA2'!$C$4:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11938,26 +11941,26 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>-0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>-0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25</c:v>
+                  <c:v>-1.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.125</c:v>
+                  <c:v>-3.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'AA2'!$O$4:$O$9</c:f>
+              <c:f>'AA2'!$J$4:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -11965,19 +11968,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.1027801090608698</c:v>
+                  <c:v>-4.150623006427314E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47769005221647298</c:v>
+                  <c:v>-7.1962899803211704E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.69736262358078105</c:v>
+                  <c:v>1.2679017669461411E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.261952708136423</c:v>
+                  <c:v>-2.93194539904322E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.079356636426406</c:v>
+                  <c:v>0.17154266269778329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11985,7 +11988,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0FFA-4716-84CB-F1D5048600B4}"/>
+              <c16:uniqueId val="{00000000-D701-49B1-AC14-4C0D047C1943}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -11993,7 +11996,7 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>90 deg</c:v>
+            <c:v>Curv. Y (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -12019,7 +12022,31 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'AA2'!$D$10:$D$15</c:f>
+              <c:f>'AA2'!$B$11:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'AA2'!$K$10:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -12027,46 +12054,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>-3.6991606287286587E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>1.0205438952445941E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>1.339855022400281E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25</c:v>
+                  <c:v>-3.4371310673939927E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'AA2'!$O$10:$O$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.8389009823434108</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.69789866642315967</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.73769809232086292</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.4679837400661879</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.3524820839609021E-2</c:v>
+                  <c:v>-4.639079019703527E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12074,7 +12074,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0FFA-4716-84CB-F1D5048600B4}"/>
+              <c16:uniqueId val="{00000001-D701-49B1-AC14-4C0D047C1943}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12234,19 +12234,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Arg Error (degs)</a:t>
+                  <a:t>Predicted Curvature Error (1/m)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="2.7777777777777776E-2"/>
-              <c:y val="0.33374999999999999"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12550,7 +12542,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-04B6-45D4-903A-9A2BE70E4EE8}"/>
+              <c16:uniqueId val="{00000000-B447-4A59-A298-CF56F83DE80E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12675,7 +12667,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-04B6-45D4-903A-9A2BE70E4EE8}"/>
+              <c16:uniqueId val="{00000001-B447-4A59-A298-CF56F83DE80E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13143,7 +13135,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B065-40A9-A92A-E90AA51B1B74}"/>
+              <c16:uniqueId val="{00000000-8474-4D0E-B20D-7D56AF492FCB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13268,7 +13260,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B065-40A9-A92A-E90AA51B1B74}"/>
+              <c16:uniqueId val="{00000001-8474-4D0E-B20D-7D56AF492FCB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13736,7 +13728,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-67DB-46B3-B007-9C8DDC879682}"/>
+              <c16:uniqueId val="{00000000-557D-45BC-85FF-A0DBB6D526C8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13861,7 +13853,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-67DB-46B3-B007-9C8DDC879682}"/>
+              <c16:uniqueId val="{00000001-557D-45BC-85FF-A0DBB6D526C8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -14940,7 +14932,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-47CD-4484-8CF9-1C06C71ABAC6}"/>
+              <c16:uniqueId val="{00000000-F726-4BC9-A251-78EF8B8426F4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15029,7 +15021,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-47CD-4484-8CF9-1C06C71ABAC6}"/>
+              <c16:uniqueId val="{00000001-F726-4BC9-A251-78EF8B8426F4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15118,7 +15110,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-47CD-4484-8CF9-1C06C71ABAC6}"/>
+              <c16:uniqueId val="{00000002-F726-4BC9-A251-78EF8B8426F4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15207,7 +15199,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-47CD-4484-8CF9-1C06C71ABAC6}"/>
+              <c16:uniqueId val="{00000003-F726-4BC9-A251-78EF8B8426F4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15693,7 +15685,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3C2F-4A58-81A2-305F326FD8C5}"/>
+              <c16:uniqueId val="{00000000-A1FD-4E0D-AE3C-87D5987DD983}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15782,7 +15774,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3C2F-4A58-81A2-305F326FD8C5}"/>
+              <c16:uniqueId val="{00000001-A1FD-4E0D-AE3C-87D5987DD983}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15868,7 +15860,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3C2F-4A58-81A2-305F326FD8C5}"/>
+              <c16:uniqueId val="{00000002-A1FD-4E0D-AE3C-87D5987DD983}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -15957,7 +15949,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-3C2F-4A58-81A2-305F326FD8C5}"/>
+              <c16:uniqueId val="{00000003-A1FD-4E0D-AE3C-87D5987DD983}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -16448,7 +16440,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6460-4221-AE6A-064FD82801A5}"/>
+              <c16:uniqueId val="{00000000-9BFC-471D-8DB9-5126E0D47C2F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -16537,7 +16529,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6460-4221-AE6A-064FD82801A5}"/>
+              <c16:uniqueId val="{00000001-9BFC-471D-8DB9-5126E0D47C2F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -16626,7 +16618,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-6460-4221-AE6A-064FD82801A5}"/>
+              <c16:uniqueId val="{00000002-9BFC-471D-8DB9-5126E0D47C2F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -16715,7 +16707,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-6460-4221-AE6A-064FD82801A5}"/>
+              <c16:uniqueId val="{00000003-9BFC-471D-8DB9-5126E0D47C2F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -17201,7 +17193,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5D0E-4A31-8D94-CCA4BDE18714}"/>
+              <c16:uniqueId val="{00000000-BC50-4916-BE67-553859E30B15}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -17290,7 +17282,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5D0E-4A31-8D94-CCA4BDE18714}"/>
+              <c16:uniqueId val="{00000001-BC50-4916-BE67-553859E30B15}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -17766,7 +17758,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F5C2-4601-9ADC-67238ED3BF2E}"/>
+              <c16:uniqueId val="{00000000-6EA9-4782-A13A-593AB429FC9F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -17891,7 +17883,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F5C2-4601-9ADC-67238ED3BF2E}"/>
+              <c16:uniqueId val="{00000001-6EA9-4782-A13A-593AB429FC9F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -18359,7 +18351,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-03D7-473D-96B5-DEF16CDAEA63}"/>
+              <c16:uniqueId val="{00000000-EE1E-49F4-BF19-8A7BC8CBB7D7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -18484,7 +18476,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-03D7-473D-96B5-DEF16CDAEA63}"/>
+              <c16:uniqueId val="{00000001-EE1E-49F4-BF19-8A7BC8CBB7D7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -18932,7 +18924,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E0EF-4E28-9885-14453FDDF02C}"/>
+              <c16:uniqueId val="{00000000-FAD0-47BE-A324-C190AF73F334}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -19021,7 +19013,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E0EF-4E28-9885-14453FDDF02C}"/>
+              <c16:uniqueId val="{00000001-FAD0-47BE-A324-C190AF73F334}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -19097,7 +19089,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E0EF-4E28-9885-14453FDDF02C}"/>
+              <c16:uniqueId val="{00000002-FAD0-47BE-A324-C190AF73F334}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -19507,7 +19499,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-847E-400C-BF7E-B512155F74FA}"/>
+              <c16:uniqueId val="{00000000-F484-4EBF-9C59-13CC5DA35D0A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -19596,7 +19588,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-847E-400C-BF7E-B512155F74FA}"/>
+              <c16:uniqueId val="{00000001-F484-4EBF-9C59-13CC5DA35D0A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -19685,7 +19677,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-847E-400C-BF7E-B512155F74FA}"/>
+              <c16:uniqueId val="{00000002-F484-4EBF-9C59-13CC5DA35D0A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -19774,7 +19766,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-847E-400C-BF7E-B512155F74FA}"/>
+              <c16:uniqueId val="{00000003-F484-4EBF-9C59-13CC5DA35D0A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -20186,7 +20178,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Curv. Y (0 deg)</c:v>
+            <c:v>Curv. Y (In-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -20267,7 +20259,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CB5B-4BD4-AE8B-16E00E4472EA}"/>
+              <c16:uniqueId val="{00000000-53D4-48CC-9D0F-979075695846}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -20275,7 +20267,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Curv. X (0 deg)</c:v>
+            <c:v>Curv. X (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -20356,15 +20348,104 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CB5B-4BD4-AE8B-16E00E4472EA}"/>
+              <c16:uniqueId val="{00000001-53D4-48CC-9D0F-979075695846}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Curv. X (In-Plane)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'AA3'!$B$10:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'AA3'!$J$10:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2038067948810856E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16581659997185549</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22516722739193451</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21758748134009179</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-3.5663418157071643E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-53D4-48CC-9D0F-979075695846}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
-            <c:v>Curv. Y (90 deg)</c:v>
+            <c:v>Curv. Y (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -20442,96 +20523,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-CB5B-4BD4-AE8B-16E00E4472EA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Curv. X (90 deg)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'AA3'!$B$10:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'AA3'!$J$10:$J$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.2038067948810856E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.16581659997185549</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.22516722739193451</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.21758748134009179</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-3.5663418157071643E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-CB5B-4BD4-AE8B-16E00E4472EA}"/>
+              <c16:uniqueId val="{00000003-53D4-48CC-9D0F-979075695846}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -20884,7 +20876,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Angular</a:t>
+              <a:t>Curvature</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -20892,8 +20884,15 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>: Predicted vs. Actual</a:t>
+              <a:t>: </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Out-of-Plane</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -20933,13 +20932,13 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>0 deg</c:v>
+            <c:v>Curv. X (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -20950,11 +20949,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -20962,7 +20961,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'AA3'!$D$4:$D$9</c:f>
+              <c:f>'AA3'!$C$4:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -20970,26 +20969,26 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>-0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>-0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25</c:v>
+                  <c:v>-1.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.125</c:v>
+                  <c:v>-3.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'AA3'!$O$4:$O$9</c:f>
+              <c:f>'AA3'!$J$4:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -20997,19 +20996,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.50828807571715</c:v>
+                  <c:v>-6.4442738072131522E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.1493134717745</c:v>
+                  <c:v>-0.15618364865216561</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.64962967046023</c:v>
+                  <c:v>-0.2055441289920476</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.327526375061896</c:v>
+                  <c:v>-6.5684533074740314E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.91856232635227042</c:v>
+                  <c:v>5.0141639433203787E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21017,7 +21016,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C7CA-42C4-BFC1-57140A598096}"/>
+              <c16:uniqueId val="{00000000-8489-45B1-A454-DA446B0D9F5B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -21025,7 +21024,7 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>90 deg</c:v>
+            <c:v>Curv. Y (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -21051,7 +21050,31 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'AA3'!$D$10:$D$15</c:f>
+              <c:f>'AA3'!$B$11:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'AA3'!$K$10:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -21059,46 +21082,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>-7.9596437042579057E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>-0.1735261696614992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>-0.19387043930777559</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25</c:v>
+                  <c:v>-3.508084274548566E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'AA3'!$O$10:$O$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>25.356071877770159</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.302792589800831</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.04753463217857</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.9461321427334961</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.64859985504053408</c:v>
+                  <c:v>3.5780879920351741E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21106,7 +21102,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C7CA-42C4-BFC1-57140A598096}"/>
+              <c16:uniqueId val="{00000001-8489-45B1-A454-DA446B0D9F5B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -21266,19 +21262,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Arg Error (degs)</a:t>
+                  <a:t>Predicted Curvature Error (1/m)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="2.7777777777777776E-2"/>
-              <c:y val="0.3383796296296297"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -22335,7 +22323,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-777B-423B-9F7E-CFBB3FC69C42}"/>
+              <c16:uniqueId val="{00000000-634F-4983-83F5-C8B9BD167A7C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -22460,7 +22448,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-777B-423B-9F7E-CFBB3FC69C42}"/>
+              <c16:uniqueId val="{00000001-634F-4983-83F5-C8B9BD167A7C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -22928,7 +22916,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7310-424E-9FE2-D4DA7FF61B8B}"/>
+              <c16:uniqueId val="{00000000-EE86-43B8-A57A-9854D7A34ED2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -23053,7 +23041,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7310-424E-9FE2-D4DA7FF61B8B}"/>
+              <c16:uniqueId val="{00000001-EE86-43B8-A57A-9854D7A34ED2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -23521,7 +23509,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F44C-484A-8A7A-1F51CE52D6DF}"/>
+              <c16:uniqueId val="{00000000-AC2C-4B61-BA54-E231B2388005}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -23646,7 +23634,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F44C-484A-8A7A-1F51CE52D6DF}"/>
+              <c16:uniqueId val="{00000001-AC2C-4B61-BA54-E231B2388005}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -24132,7 +24120,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-66C7-46B7-85C1-6831732605A1}"/>
+              <c16:uniqueId val="{00000000-F876-4A3E-8A9C-1A2F9D7E0ACF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -24221,7 +24209,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-66C7-46B7-85C1-6831732605A1}"/>
+              <c16:uniqueId val="{00000001-F876-4A3E-8A9C-1A2F9D7E0ACF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -24310,7 +24298,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-66C7-46B7-85C1-6831732605A1}"/>
+              <c16:uniqueId val="{00000002-F876-4A3E-8A9C-1A2F9D7E0ACF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -24399,7 +24387,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-66C7-46B7-85C1-6831732605A1}"/>
+              <c16:uniqueId val="{00000003-F876-4A3E-8A9C-1A2F9D7E0ACF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -24885,7 +24873,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3C68-44A6-915A-79483435386A}"/>
+              <c16:uniqueId val="{00000000-315A-4272-9E66-2559FE7BE243}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -24974,7 +24962,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-3C68-44A6-915A-79483435386A}"/>
+              <c16:uniqueId val="{00000001-315A-4272-9E66-2559FE7BE243}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -25060,7 +25048,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3C68-44A6-915A-79483435386A}"/>
+              <c16:uniqueId val="{00000002-315A-4272-9E66-2559FE7BE243}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -25149,7 +25137,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-3C68-44A6-915A-79483435386A}"/>
+              <c16:uniqueId val="{00000003-315A-4272-9E66-2559FE7BE243}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -25640,7 +25628,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-84B5-45B3-B7EA-2F69CE2B447C}"/>
+              <c16:uniqueId val="{00000000-6BB2-4B35-9034-07CEA3B9C5AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -25729,7 +25717,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-84B5-45B3-B7EA-2F69CE2B447C}"/>
+              <c16:uniqueId val="{00000001-6BB2-4B35-9034-07CEA3B9C5AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -25818,7 +25806,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-84B5-45B3-B7EA-2F69CE2B447C}"/>
+              <c16:uniqueId val="{00000002-6BB2-4B35-9034-07CEA3B9C5AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -25907,7 +25895,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-84B5-45B3-B7EA-2F69CE2B447C}"/>
+              <c16:uniqueId val="{00000003-6BB2-4B35-9034-07CEA3B9C5AC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -26393,7 +26381,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-763C-469D-9FF1-5F04CB0240AA}"/>
+              <c16:uniqueId val="{00000000-5B57-4EB2-AD06-B2523B377E8D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -26482,7 +26470,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-763C-469D-9FF1-5F04CB0240AA}"/>
+              <c16:uniqueId val="{00000001-5B57-4EB2-AD06-B2523B377E8D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -26958,7 +26946,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F4DB-4E18-A0BC-57D671C73EF8}"/>
+              <c16:uniqueId val="{00000000-9479-4650-BFD6-DA174C42D566}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -27083,7 +27071,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F4DB-4E18-A0BC-57D671C73EF8}"/>
+              <c16:uniqueId val="{00000001-9479-4650-BFD6-DA174C42D566}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -27551,7 +27539,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6EC0-4005-9E18-C019DA2360DF}"/>
+              <c16:uniqueId val="{00000000-5F99-48AF-A5AA-D13CE76E8613}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -27676,7 +27664,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6EC0-4005-9E18-C019DA2360DF}"/>
+              <c16:uniqueId val="{00000001-5F99-48AF-A5AA-D13CE76E8613}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -28124,7 +28112,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CEB4-41F3-BA8C-8647DD180618}"/>
+              <c16:uniqueId val="{00000000-7DB5-4E29-9456-AD5B66B6C3CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -28213,7 +28201,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CEB4-41F3-BA8C-8647DD180618}"/>
+              <c16:uniqueId val="{00000001-7DB5-4E29-9456-AD5B66B6C3CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -28289,7 +28277,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-CEB4-41F3-BA8C-8647DD180618}"/>
+              <c16:uniqueId val="{00000002-7DB5-4E29-9456-AD5B66B6C3CB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -29324,21 +29312,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Curvature</a:t>
+              <a:t>Curvature Error: Magnitude Error</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Error</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>: Magnitude</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Error</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -29462,7 +29437,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FBDC-47D7-84CA-91346EA78596}"/>
+              <c16:uniqueId val="{00000000-1269-4975-9FC7-2C7F8DB372E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -29551,7 +29526,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FBDC-47D7-84CA-91346EA78596}"/>
+              <c16:uniqueId val="{00000001-1269-4975-9FC7-2C7F8DB372E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -29640,7 +29615,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FBDC-47D7-84CA-91346EA78596}"/>
+              <c16:uniqueId val="{00000002-1269-4975-9FC7-2C7F8DB372E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -29729,7 +29704,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-FBDC-47D7-84CA-91346EA78596}"/>
+              <c16:uniqueId val="{00000003-1269-4975-9FC7-2C7F8DB372E6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -30086,7 +30061,17 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Error: Component Error</a:t>
+              <a:t> Error</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>: </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Component Error</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -30131,7 +30116,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Curv. Y (0 deg)</c:v>
+            <c:v>Curv. Y (In-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -30212,7 +30197,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8837-4347-BCD4-9D4A7F5B720F}"/>
+              <c16:uniqueId val="{00000000-75AB-49FC-9A2B-660B1D93EAE0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -30220,7 +30205,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Curv. X (0 deg)</c:v>
+            <c:v>Curv. X (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -30301,15 +30286,104 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8837-4347-BCD4-9D4A7F5B720F}"/>
+              <c16:uniqueId val="{00000001-75AB-49FC-9A2B-660B1D93EAE0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Curv. X (In-Plane)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'AA4'!$B$10:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'AA4'!$J$10:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1125916087597333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30338583845926109</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.42633814699968442</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.62337605053123335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.439762313669924</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-75AB-49FC-9A2B-660B1D93EAE0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
-            <c:v>Curv. Y (90 deg)</c:v>
+            <c:v>Curv. Y (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -30387,96 +30461,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8837-4347-BCD4-9D4A7F5B720F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Curv. X (90 deg)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'AA4'!$B$10:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'AA4'!$J$10:$J$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.1125916087597333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.30338583845926109</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.42633814699968442</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.62337605053123335</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.439762313669924</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8837-4347-BCD4-9D4A7F5B720F}"/>
+              <c16:uniqueId val="{00000003-75AB-49FC-9A2B-660B1D93EAE0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -30829,7 +30814,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Angular</a:t>
+              <a:t>Curvature</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -30837,8 +30822,15 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>: Predicted vs. Actual</a:t>
+              <a:t>: </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Out-of-Plane</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -30878,13 +30870,13 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>0 deg</c:v>
+            <c:v>Curv. X (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -30895,11 +30887,11 @@
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent2"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -30907,7 +30899,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'AA4'!$D$4:$D$9</c:f>
+              <c:f>'AA4'!$C$4:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -30915,26 +30907,26 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>-0.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>-0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25</c:v>
+                  <c:v>-1.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.125</c:v>
+                  <c:v>-3.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'AA4'!$O$4:$O$9</c:f>
+              <c:f>'AA4'!$J$4:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -30942,19 +30934,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>121.3666700117961</c:v>
+                  <c:v>-4.0434754872752547E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.9007916169639052</c:v>
+                  <c:v>1.156419375414189E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.660671184508729</c:v>
+                  <c:v>-8.5710139811272651E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-24.055088476500899</c:v>
+                  <c:v>0.27129931550231701</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-21.933383331331441</c:v>
+                  <c:v>0.74842091378218967</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -30962,7 +30954,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CA27-49A8-9912-57703CA86D83}"/>
+              <c16:uniqueId val="{00000000-8B7C-429E-B97A-722914F77A60}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -30970,7 +30962,7 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>90 deg</c:v>
+            <c:v>Curv. Y (Out-of-Plane)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -30996,7 +30988,31 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'AA4'!$D$10:$D$15</c:f>
+              <c:f>'AA4'!$B$11:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'AA4'!$K$10:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -31004,46 +31020,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25</c:v>
+                  <c:v>-0.18886458206208179</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.8</c:v>
+                  <c:v>-0.66056585894506348</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>-0.76523888557143305</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.25</c:v>
+                  <c:v>-0.80017185550318626</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'AA4'!$O$10:$O$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>53.962244348190268</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>53.064113129393142</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>53.14291372238597</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>51.935088355649853</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>48.908156704592983</c:v>
+                  <c:v>-1.9323794909329699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -31051,7 +31040,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CA27-49A8-9912-57703CA86D83}"/>
+              <c16:uniqueId val="{00000001-8B7C-429E-B97A-722914F77A60}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -31211,19 +31200,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Arg Error (degs)</a:t>
+                  <a:t>Predicted Curvature Error (1/m)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="2.7777777777777776E-2"/>
-              <c:y val="0.3244907407407408"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -60784,16 +60765,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>94384</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>170584</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -60822,16 +60803,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -60973,15 +60954,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>121227</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>63211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>664152</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>139411</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -61048,23 +61029,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>442479</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>6927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>83994</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>83127</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="15" name="Chart 14">
+        <xdr:cNvPr id="16" name="Chart 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CDFFD85-1C74-454C-B9E6-29DF6305676E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4730B118-382A-4997-90C3-EA28AC9C0999}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61107,7 +61088,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97BB6C5A-BB68-4053-B75F-63E2FFCF99F6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A37F0B5D-D0CC-4A01-B502-3FD37596211E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61145,7 +61126,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A55772CA-0EFA-4924-B1D4-399E2099F13D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E83740F-7EFE-4815-9D07-B208F1111A78}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61183,7 +61164,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{985A3172-1843-4358-A574-09877D65971E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A4B1908-4B70-4927-A6D6-9640CFA67BDE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61221,7 +61202,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4275199C-95F5-4967-BE9E-90DC554B0515}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC697FFA-77E8-4930-8473-010476ED9B5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61259,7 +61240,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1F48380-AAA5-4361-A27B-E9FA0FB03229}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D6B9FA-73D5-4310-8826-38EBC9069D0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61281,23 +61262,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>94384</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>170584</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79AFA359-D95F-448F-9F19-2C1699F5329E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9284B041-7F72-466B-A9DF-F22B17A3A596}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61319,23 +61300,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28EE727D-770E-4B25-BA8D-F9BE29761690}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3893953E-9003-4914-B799-BD4D784F9B13}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61373,7 +61354,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E27F1BD-0CD0-4100-8893-1184FF74AF43}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B62B3FD-45A8-4669-A92B-1D5F60AA32A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61411,7 +61392,7 @@
         <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{589B8AAD-3B60-4751-9A50-6FEAE4797A3F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D352E552-7B84-4270-9B30-18EDD17C9457}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61449,7 +61430,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A78638D-E621-451D-98DA-F48EE8AB3278}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{973B47D0-04CC-4D29-B35F-67E8410B848D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61472,22 +61453,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>121227</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>63211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>664152</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>139411</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="12" name="Chart 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2B1F91C-C794-4863-A7E7-9B80299ABEA9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47BCC39B-9850-468D-A104-BE7306A09720}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61525,7 +61506,7 @@
         <xdr:cNvPr id="13" name="Chart 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44E5E723-F53F-44FC-81F8-D6CB5D4219E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D9440E8-4FFE-45BC-AAD8-3A451EBF4F37}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61547,23 +61528,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>442479</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>6927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>83994</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>83127</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="14" name="Chart 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{867C7E40-21B6-4244-A197-8C3440D846E2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF2D8BF2-2DE4-4F8D-8D41-566918C07333}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61606,7 +61587,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F82E337-284A-4AF2-8D63-5D95B7E3B8DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFC9C5DE-CF82-4180-BEBE-656F7F6A4C1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61644,7 +61625,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{510215EE-6196-4BFC-83DA-2ADF5E1BBD06}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC69364-41AF-4ED3-BE97-E13217CBA403}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61682,7 +61663,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AA6EA16-A596-46E3-BE2A-9971C9706C20}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB4CAF6F-6460-4176-BA6B-A2AD3D0DB550}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61720,7 +61701,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28429EC7-08CC-4ABC-800B-10F6720B4D8C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46F5CB8C-8218-4E1A-8612-6420830948E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61758,7 +61739,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD7BB0A0-A71F-417E-BD5B-3009C3655808}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3379A0FE-6CEF-4CD0-AB7D-E3F0A8F18DA0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61780,23 +61761,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>94384</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>170584</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC322F5-CC9E-4313-96A0-9633911A122F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECEAA48C-4555-4308-BD91-AFE45CF21A95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61818,23 +61799,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{089E44C4-4E9D-4D92-AAFF-914D68A71322}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{842CD861-DD05-4D55-9427-A8A3AD0F01B3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61872,7 +61853,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34981F7B-AAC7-40BA-B536-3C7C75499FFD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12ECB48B-A8E6-4DF3-92B2-2D8E5D374CFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61910,7 +61891,7 @@
         <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38D570AB-5EB7-4C36-87B3-66B84FB81F60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4AA9224-FFAD-4C34-AFF2-C3B67F0B9AB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61948,7 +61929,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6440F98-006C-40F8-BEC1-76741E2A4DED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5FE07D0-7E05-44FE-B965-1565437D9412}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -61971,22 +61952,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>121227</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>63211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>664152</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>139411</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="12" name="Chart 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9568C7BC-3C2A-44AE-BA29-596DBCB2048C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3E1A924-B901-433A-8D6C-2CA393958DC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62024,7 +62005,7 @@
         <xdr:cNvPr id="13" name="Chart 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE41743B-B6A7-4990-A549-2EF3A7466F55}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53229CE8-DDFA-4CFC-B6EC-8D1ADB7AEAD5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62046,23 +62027,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>442479</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>6927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>83994</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>83127</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="14" name="Chart 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A283705-74E8-4513-A180-13F68A2597C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D986CE0-3A58-49B8-8B13-42796F0EF12C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62105,7 +62086,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B125EE88-4B6E-4296-80E3-8A0E39D49CA3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{822D8B82-877E-4877-9A72-9F5D4DB67A17}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62143,7 +62124,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{105AE94E-A1F1-4004-8DA1-449E0E6C9083}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C5526FB-A6E8-4641-B37F-FED0BB920811}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62181,7 +62162,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F3724C4-D597-4F0F-B203-E8641D65D35E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CD244CF-0167-492D-9674-786301EBB4F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62219,7 +62200,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8BD316A-40AF-407B-BB4E-529E15BADAA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4172C3C7-4001-4584-A165-D9E1C3A59660}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62257,7 +62238,7 @@
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF52CA6D-6910-457B-BA4E-EE4C722A2A7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F48DF826-1D70-4FA4-A308-5A81C2532E02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62279,23 +62260,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>94384</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>170584</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CB9CD9A-84E3-47E7-8505-E8B6AAC3DD6E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E9835B5-52AF-4E8F-B6FA-C65F12BEFA8B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62317,23 +62298,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ABB78D6-72AC-4256-8D0D-B12B3B8B14C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42CB1112-ADC1-43E6-8A99-B9490A65BC73}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62371,7 +62352,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{750FFA15-7BC3-4C78-A5E9-3B7D0027229C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{017283C0-CC62-4F08-B928-F693713142F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62409,7 +62390,7 @@
         <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5388258F-51A2-411C-A40A-C5059E599F3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB61815F-F982-4DDD-B1A3-FB6F67DA6E1E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62447,7 +62428,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BD168D2-5F4D-4EE7-A55D-7BCECC771B82}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{250DA919-AC4B-462C-9EAD-49B66AB2B5F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62470,22 +62451,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>121227</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>63211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>664152</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>139411</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="12" name="Chart 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE5084ED-DCE4-443C-AE8F-E95CE2137FC4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6F8F42A-97E5-4A25-A22E-440C813FE55F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62523,7 +62504,7 @@
         <xdr:cNvPr id="13" name="Chart 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE86E887-EFAA-4959-90C1-BFD97EFAB1EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C05E8ADE-51A7-441F-9ED0-EE70E005F15D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62545,23 +62526,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>442479</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>6927</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>83994</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>83127</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="14" name="Chart 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABDE8D12-51D2-44E2-8193-EAF6C83FC348}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40E92D1D-ABA0-4C6C-9CB8-DA0C4054205A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -62907,8 +62888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:O15"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63567,11 +63548,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3B7FAB-FA3E-493D-B0D2-5E3BA52F212C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E7D690-F674-43C7-B419-833593222DE5}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:O15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64230,11 +64211,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28EB4477-512C-41A7-945E-C0DFAA3E9266}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED849DFB-4B0E-4059-8753-2F4E960EA12D}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:O15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64893,11 +64874,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA35ED8-35B7-4084-A62D-2DBB4A594E46}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C82B0F-4BB3-4B62-93F2-9309E7EE8C54}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:O15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>